<commit_message>
add autocheckout and 3 latest zip available on employee view
</commit_message>
<xml_diff>
--- a/Backend/Copy of Data_Base_Karyawan_Upload_System(2) - Copy.xlsx
+++ b/Backend/Copy of Data_Base_Karyawan_Upload_System(2) - Copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Tugas Zikri\Semester 6\Magang Chateraise\HRIS II\HRIS\Backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\Tugas Zikri\Semester 6\Magang Chateraise\HRIS II\BARU\HRIS\Backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D488C6AD-5797-4989-B603-5506041E0D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C310E012-37B3-4FD6-A987-F9171ED9B0A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12516" yWindow="2532" windowWidth="10620" windowHeight="9420" xr2:uid="{73AFAB64-D02A-4053-B1E0-4A252B5D9588}"/>
+    <workbookView xWindow="3384" yWindow="3384" windowWidth="10620" windowHeight="9420" xr2:uid="{73AFAB64-D02A-4053-B1E0-4A252B5D9588}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="435">
   <si>
     <t>No</t>
   </si>
@@ -183,15 +183,6 @@
     <t>087777102138</t>
   </si>
   <si>
-    <t xml:space="preserve">cocoerlangga81@gmail.com </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMK SEDERAJAT </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMK MANUNGGAL CIBINONG </t>
-  </si>
-  <si>
     <t>Pabuaran indah blok f2 no.8 rt05/05 Cibinong Bogor</t>
   </si>
   <si>
@@ -1342,6 +1333,12 @@
   </si>
   <si>
     <t>G</t>
+  </si>
+  <si>
+    <t>SMK MANUNGGAL CIBINONG</t>
+  </si>
+  <si>
+    <t>cocoerlangga81@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -1515,9 +1512,6 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1592,6 +1586,9 @@
     </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1910,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90625332-1E54-49E1-B6AB-A8249AECD88C}">
   <dimension ref="A1:Z42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1942,10 +1939,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -1975,7 +1972,7 @@
         <v>10</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="O1" s="3" t="s">
         <v>11</v>
@@ -2010,8 +2007,8 @@
       <c r="Y1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="44" t="s">
-        <v>388</v>
+      <c r="Z1" s="43" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2032,11 +2029,11 @@
       <c r="E2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="45">
+      <c r="F2" s="44">
         <v>44368</v>
       </c>
       <c r="G2" s="17"/>
-      <c r="H2" s="48">
+      <c r="H2" s="47">
         <v>35359</v>
       </c>
       <c r="I2" s="3" t="s">
@@ -2059,7 +2056,7 @@
         <v>46</v>
       </c>
       <c r="O2" s="19" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="P2" s="3" t="s">
         <v>47</v>
@@ -2069,26 +2066,26 @@
       <c r="S2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="T2" s="21" t="s">
-        <v>49</v>
+      <c r="T2" s="48" t="s">
+        <v>434</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>51</v>
+        <v>433</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="X2" s="3">
         <v>2015</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="Z2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2109,24 +2106,24 @@
       <c r="E3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="F3" s="45">
+      <c r="F3" s="44">
         <v>44536</v>
       </c>
       <c r="G3" s="17"/>
-      <c r="H3" s="48">
+      <c r="H3" s="47">
         <v>35294</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="K3" s="13">
         <v>3301133012100010</v>
       </c>
       <c r="L3" s="19" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="M3" s="19" t="str">
         <f>IF(LOWER(N3)="l","male",IF(LOWER(N3)="p","female",""))</f>
@@ -2136,7 +2133,7 @@
         <v>46</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="P3" s="3"/>
       <c r="Q3" s="3">
@@ -2144,28 +2141,28 @@
       </c>
       <c r="R3" s="3"/>
       <c r="S3" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="T3" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="T3" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="X3" s="3">
         <v>2014</v>
       </c>
       <c r="Y3" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="Z3" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2186,24 +2183,24 @@
       <c r="E4" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="45">
+      <c r="F4" s="44">
         <v>44536</v>
       </c>
       <c r="G4" s="17"/>
-      <c r="H4" s="48">
+      <c r="H4" s="47">
         <v>34766</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="K4" s="13">
         <v>1275012311210000</v>
       </c>
       <c r="L4" s="19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M4" s="19" t="str">
         <f t="shared" ref="M4:M42" si="1">IF(LOWER(N4)="l","male",IF(LOWER(N4)="p","female",""))</f>
@@ -2213,7 +2210,7 @@
         <v>46</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="P4" s="3"/>
       <c r="Q4" s="3">
@@ -2221,28 +2218,28 @@
       </c>
       <c r="R4" s="3"/>
       <c r="S4" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="T4" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="V4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="W4" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="T4" s="22" t="s">
-        <v>65</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="W4" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="X4" s="3">
         <v>2013</v>
       </c>
       <c r="Y4" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Z4" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2263,57 +2260,57 @@
       <c r="E5" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="45">
+      <c r="F5" s="44">
         <v>44733</v>
       </c>
       <c r="G5" s="17"/>
-      <c r="H5" s="45">
+      <c r="H5" s="44">
         <v>38123</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="K5" s="23">
+        <v>67</v>
+      </c>
+      <c r="K5" s="22">
         <v>3201031505090020</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="M5" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N5" s="24" t="s">
+      <c r="N5" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-      <c r="S5" s="25" t="s">
-        <v>72</v>
+      <c r="S5" s="24" t="s">
+        <v>69</v>
       </c>
       <c r="T5" s="16"/>
       <c r="U5" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="X5" s="2">
         <v>2022</v>
       </c>
       <c r="Y5" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="Z5" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2334,59 +2331,59 @@
       <c r="E6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="45">
+      <c r="F6" s="44">
         <v>44733</v>
       </c>
       <c r="G6" s="17"/>
-      <c r="H6" s="45">
+      <c r="H6" s="44">
         <v>38075</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>43</v>
       </c>
       <c r="J6" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="K6" s="25" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="K6" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="M6" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N6" s="24" t="s">
+      <c r="N6" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-      <c r="S6" s="25" t="s">
-        <v>80</v>
-      </c>
-      <c r="T6" s="22" t="s">
-        <v>81</v>
+      <c r="S6" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="T6" s="21" t="s">
+        <v>78</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V6" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="W6" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="X6" s="2">
         <v>2022</v>
       </c>
       <c r="Y6" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="Z6" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2407,61 +2404,61 @@
       <c r="E7" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="45">
+      <c r="F7" s="44">
         <v>44733</v>
       </c>
       <c r="G7" s="17"/>
-      <c r="H7" s="45">
+      <c r="H7" s="44">
         <v>37874</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="K7" s="23">
+        <v>80</v>
+      </c>
+      <c r="K7" s="22">
         <v>3201030907100020</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M7" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N7" s="24" t="s">
+      <c r="N7" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-      <c r="S7" s="25" t="s">
-        <v>86</v>
+      <c r="S7" s="24" t="s">
+        <v>83</v>
       </c>
       <c r="T7" s="16"/>
       <c r="U7" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="X7" s="2">
         <v>2022</v>
       </c>
       <c r="Y7" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="Z7" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2482,59 +2479,59 @@
       <c r="E8" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="45">
+      <c r="F8" s="44">
         <v>44733</v>
       </c>
       <c r="G8" s="17"/>
-      <c r="H8" s="45">
+      <c r="H8" s="44">
         <v>37042</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="K8" s="23">
+        <v>85</v>
+      </c>
+      <c r="K8" s="22">
         <v>3201030609180000</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="M8" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N8" s="24" t="s">
+      <c r="N8" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-      <c r="S8" s="25" t="s">
+      <c r="S8" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="T8" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="V8" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="T8" s="22" t="s">
+      <c r="W8" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="U8" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="V8" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="W8" s="3" t="s">
-        <v>94</v>
       </c>
       <c r="X8" s="2">
         <v>2019</v>
       </c>
       <c r="Y8" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="Z8" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2555,59 +2552,59 @@
       <c r="E9" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="45">
+      <c r="F9" s="44">
         <v>44733</v>
       </c>
       <c r="G9" s="17"/>
-      <c r="H9" s="45">
+      <c r="H9" s="44">
         <v>38211</v>
       </c>
       <c r="I9" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="L9" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="K9" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="L9" s="4" t="s">
-        <v>99</v>
       </c>
       <c r="M9" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N9" s="24" t="s">
+      <c r="N9" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O9" s="2"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-      <c r="S9" s="25" t="s">
-        <v>100</v>
-      </c>
-      <c r="T9" s="22" t="s">
-        <v>101</v>
+      <c r="S9" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="T9" s="21" t="s">
+        <v>98</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="X9" s="2">
         <v>2022</v>
       </c>
       <c r="Y9" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="Z9" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2628,59 +2625,59 @@
       <c r="E10" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="45">
+      <c r="F10" s="44">
         <v>44733</v>
       </c>
       <c r="G10" s="17"/>
-      <c r="H10" s="45">
+      <c r="H10" s="44">
         <v>38058</v>
       </c>
       <c r="I10" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="K10" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="L10" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="K10" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="L10" s="4" t="s">
-        <v>106</v>
       </c>
       <c r="M10" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N10" s="24" t="s">
+      <c r="N10" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-      <c r="S10" s="25" t="s">
-        <v>107</v>
+      <c r="S10" s="24" t="s">
+        <v>104</v>
       </c>
       <c r="T10" s="16" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="X10" s="2">
         <v>2022</v>
       </c>
       <c r="Y10" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Z10" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2688,7 +2685,7 @@
         <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C11" s="4" t="str">
         <f>D11 &amp; COUNTIF(D$2:D11,D11)</f>
@@ -2699,61 +2696,61 @@
         <v>ni</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="F11" s="45">
+        <v>108</v>
+      </c>
+      <c r="F11" s="44">
         <v>44733</v>
       </c>
       <c r="G11" s="17"/>
-      <c r="H11" s="45">
+      <c r="H11" s="44">
         <v>38073</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>43</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="K11" s="25" t="s">
-        <v>129</v>
+        <v>125</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>126</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="M11" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-      <c r="S11" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="T11" s="22" t="s">
-        <v>132</v>
+      <c r="S11" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="T11" s="21" t="s">
+        <v>129</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V11" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="X11" s="2">
         <v>2022</v>
       </c>
       <c r="Y11" s="3" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="Z11" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2761,7 +2758,7 @@
         <v>14</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C12" s="4" t="str">
         <f>D12 &amp; COUNTIF(D$2:D12,D12)</f>
@@ -2772,61 +2769,61 @@
         <v>aura</v>
       </c>
       <c r="E12" s="16" t="s">
-        <v>113</v>
-      </c>
-      <c r="F12" s="45">
+        <v>110</v>
+      </c>
+      <c r="F12" s="44">
         <v>44733</v>
       </c>
       <c r="G12" s="17"/>
-      <c r="H12" s="45">
+      <c r="H12" s="44">
         <v>38196</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>43</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="K12" s="23">
+        <v>132</v>
+      </c>
+      <c r="K12" s="22">
         <v>3271052802074230</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="M12" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N12" s="26" t="s">
+      <c r="N12" s="25" t="s">
         <v>23</v>
       </c>
       <c r="O12" s="2"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-      <c r="S12" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="T12" s="22" t="s">
-        <v>137</v>
+      <c r="S12" s="24" t="s">
+        <v>133</v>
+      </c>
+      <c r="T12" s="21" t="s">
+        <v>134</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V12" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="X12" s="2">
         <v>2022</v>
       </c>
       <c r="Y12" s="3" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="Z12" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2834,7 +2831,7 @@
         <v>15</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C13" s="4" t="str">
         <f>D13 &amp; COUNTIF(D$2:D13,D13)</f>
@@ -2845,63 +2842,63 @@
         <v>devi</v>
       </c>
       <c r="E13" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="F13" s="45">
+        <v>112</v>
+      </c>
+      <c r="F13" s="44">
         <v>44733</v>
       </c>
       <c r="G13" s="17"/>
-      <c r="H13" s="45">
+      <c r="H13" s="44">
         <v>38032</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="K13" s="25" t="s">
-        <v>140</v>
+        <v>136</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>137</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M13" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N13" s="24" t="s">
+      <c r="N13" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O13" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-      <c r="S13" s="25" t="s">
-        <v>143</v>
-      </c>
-      <c r="T13" s="22" t="s">
-        <v>144</v>
+      <c r="S13" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="T13" s="21" t="s">
+        <v>141</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V13" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="X13" s="2">
         <v>2022</v>
       </c>
       <c r="Y13" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="Z13" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2909,7 +2906,7 @@
         <v>16</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C14" s="4" t="str">
         <f>D14 &amp; COUNTIF(D$2:D14,D14)</f>
@@ -2920,61 +2917,61 @@
         <v>khuzaery</v>
       </c>
       <c r="E14" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="F14" s="45">
+        <v>114</v>
+      </c>
+      <c r="F14" s="44">
         <v>44733</v>
       </c>
       <c r="G14" s="17"/>
-      <c r="H14" s="45">
+      <c r="H14" s="44">
         <v>35476</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="K14" s="23">
+        <v>144</v>
+      </c>
+      <c r="K14" s="22">
         <v>3212080106094600</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="M14" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N14" s="24" t="s">
+      <c r="N14" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-      <c r="S14" s="25" t="s">
-        <v>150</v>
+      <c r="S14" s="24" t="s">
+        <v>147</v>
       </c>
       <c r="T14" s="16"/>
       <c r="U14" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="V14" s="3"/>
       <c r="W14" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X14" s="2">
         <v>2015</v>
       </c>
       <c r="Y14" s="3" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="Z14" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -2982,7 +2979,7 @@
         <v>17</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C15" s="4" t="str">
         <f>D15 &amp; COUNTIF(D$2:D15,D15)</f>
@@ -2993,61 +2990,61 @@
         <v>lisda</v>
       </c>
       <c r="E15" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="F15" s="45">
+        <v>116</v>
+      </c>
+      <c r="F15" s="44">
         <v>44916</v>
       </c>
       <c r="G15" s="17"/>
-      <c r="H15" s="45">
+      <c r="H15" s="44">
         <v>37630</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="J15" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="K15" s="23">
+        <v>151</v>
+      </c>
+      <c r="K15" s="22">
         <v>3271052106120110</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="M15" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N15" s="24" t="s">
+      <c r="N15" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O15" s="2"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
-      <c r="S15" s="25" t="s">
+      <c r="S15" s="24" t="s">
+        <v>153</v>
+      </c>
+      <c r="T15" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V15" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="W15" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="T15" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="V15" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="W15" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="X15" s="2">
         <v>2021</v>
       </c>
       <c r="Y15" s="3" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="Z15" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3055,71 +3052,71 @@
         <v>18</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C16" s="4" t="str">
         <f>D16 &amp; COUNTIF(D$2:D16,D16)</f>
         <v>yuningsih1</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="E16" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="F16" s="45">
+        <v>118</v>
+      </c>
+      <c r="F16" s="44">
         <v>45054</v>
       </c>
       <c r="G16" s="17"/>
-      <c r="H16" s="45">
+      <c r="H16" s="44">
         <v>38068</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>43</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>161</v>
-      </c>
-      <c r="K16" s="25" t="s">
-        <v>162</v>
+        <v>158</v>
+      </c>
+      <c r="K16" s="24" t="s">
+        <v>159</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="M16" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N16" s="24" t="s">
+      <c r="N16" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O16" s="2"/>
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-      <c r="S16" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="T16" s="22" t="s">
-        <v>165</v>
+      <c r="S16" s="24" t="s">
+        <v>161</v>
+      </c>
+      <c r="T16" s="21" t="s">
+        <v>162</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V16" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="W16" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="X16" s="2">
         <v>2023</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="Z16" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
     </row>
     <row r="17" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3127,7 +3124,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C17" s="4" t="str">
         <f>D17 &amp; COUNTIF(D$2:D17,D17)</f>
@@ -3138,57 +3135,57 @@
         <v>ahmad</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="F17" s="45">
+        <v>120</v>
+      </c>
+      <c r="F17" s="44">
         <v>45078</v>
       </c>
       <c r="G17" s="17"/>
-      <c r="H17" s="45">
+      <c r="H17" s="44">
         <v>37539</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="K17" s="23"/>
+        <v>165</v>
+      </c>
+      <c r="K17" s="22"/>
       <c r="L17" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="M17" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N17" s="24" t="s">
+      <c r="N17" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
-      <c r="S17" s="25" t="s">
-        <v>170</v>
+      <c r="S17" s="24" t="s">
+        <v>167</v>
       </c>
       <c r="T17" s="16"/>
       <c r="U17" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V17" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="W17" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="X17" s="2">
         <v>2021</v>
       </c>
       <c r="Y17" s="3" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="Z17" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
     </row>
     <row r="18" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3196,7 +3193,7 @@
         <v>20</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C18" s="4" t="str">
         <f>D18 &amp; COUNTIF(D$2:D18,D18)</f>
@@ -3207,61 +3204,61 @@
         <v>septian</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="F18" s="45">
+        <v>122</v>
+      </c>
+      <c r="F18" s="44">
         <v>45097</v>
       </c>
       <c r="G18" s="17"/>
-      <c r="H18" s="45">
+      <c r="H18" s="44">
         <v>38259</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J18" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="K18" s="25" t="s">
-        <v>173</v>
+        <v>169</v>
+      </c>
+      <c r="K18" s="24" t="s">
+        <v>170</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="M18" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N18" s="24" t="s">
+      <c r="N18" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
-      <c r="S18" s="23" t="s">
-        <v>175</v>
+      <c r="S18" s="22" t="s">
+        <v>172</v>
       </c>
       <c r="T18" s="16" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="U18" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V18" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="X18" s="2">
         <v>2023</v>
       </c>
       <c r="Y18" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="Z18" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="19" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3269,7 +3266,7 @@
         <v>21</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C19" s="4" t="str">
         <f>D19 &amp; COUNTIF(D$2:D19,D19)</f>
@@ -3280,61 +3277,61 @@
         <v>mohamad</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>127</v>
-      </c>
-      <c r="F19" s="45">
+        <v>124</v>
+      </c>
+      <c r="F19" s="44">
         <v>45103</v>
       </c>
       <c r="G19" s="17"/>
-      <c r="H19" s="45">
+      <c r="H19" s="44">
         <v>38365</v>
       </c>
       <c r="I19" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>177</v>
+      </c>
+      <c r="L19" s="4" t="s">
         <v>178</v>
-      </c>
-      <c r="J19" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="K19" s="25" t="s">
-        <v>180</v>
-      </c>
-      <c r="L19" s="4" t="s">
-        <v>181</v>
       </c>
       <c r="M19" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N19" s="24" t="s">
+      <c r="N19" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
-      <c r="S19" s="25" t="s">
-        <v>182</v>
+      <c r="S19" s="24" t="s">
+        <v>179</v>
       </c>
       <c r="T19" s="16" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V19" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="W19" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="X19" s="2">
         <v>2023</v>
       </c>
       <c r="Y19" s="3" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="Z19" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="20" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3342,7 +3339,7 @@
         <v>23</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C20" s="4" t="str">
         <f>D20 &amp; COUNTIF(D$2:D20,D20)</f>
@@ -3353,59 +3350,59 @@
         <v>archel</v>
       </c>
       <c r="E20" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="F20" s="45">
+        <v>183</v>
+      </c>
+      <c r="F20" s="44">
         <v>45191</v>
       </c>
       <c r="G20" s="17"/>
-      <c r="H20" s="45">
+      <c r="H20" s="44">
         <v>37742</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>43</v>
       </c>
       <c r="J20" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="K20" s="25" t="s">
-        <v>188</v>
+        <v>184</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>185</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="M20" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N20" s="24" t="s">
+      <c r="N20" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
-      <c r="S20" s="25" t="s">
-        <v>190</v>
+      <c r="S20" s="24" t="s">
+        <v>187</v>
       </c>
       <c r="T20" s="16"/>
       <c r="U20" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V20" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="W20" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="X20" s="2">
         <v>2021</v>
       </c>
       <c r="Y20" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="Z20" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="21" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3413,7 +3410,7 @@
         <v>25</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C21" s="4" t="str">
         <f>D21 &amp; COUNTIF(D$2:D21,D21)</f>
@@ -3424,59 +3421,59 @@
         <v>hilal</v>
       </c>
       <c r="E21" s="16" t="s">
-        <v>194</v>
-      </c>
-      <c r="F21" s="45">
+        <v>191</v>
+      </c>
+      <c r="F21" s="44">
         <v>45287</v>
       </c>
       <c r="G21" s="17"/>
-      <c r="H21" s="45">
+      <c r="H21" s="44">
         <v>36799</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>22</v>
       </c>
       <c r="J21" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="K21" s="23"/>
+        <v>192</v>
+      </c>
+      <c r="K21" s="22"/>
       <c r="L21" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="M21" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N21" s="24" t="s">
+      <c r="N21" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O21" s="2"/>
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
-      <c r="S21" s="25" t="s">
+      <c r="S21" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="T21" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V21" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="W21" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="T21" s="27" t="s">
-        <v>198</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="V21" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="W21" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="X21" s="2">
         <v>2018</v>
       </c>
       <c r="Y21" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="Z21" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="22" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3484,7 +3481,7 @@
         <v>27</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C22" s="4" t="str">
         <f>D22 &amp; COUNTIF(D$2:D22,D22)</f>
@@ -3495,67 +3492,67 @@
         <v>adlan</v>
       </c>
       <c r="E22" s="16" t="s">
-        <v>203</v>
-      </c>
-      <c r="F22" s="45">
+        <v>200</v>
+      </c>
+      <c r="F22" s="44">
         <v>45301</v>
       </c>
       <c r="G22" s="17"/>
-      <c r="H22" s="45">
+      <c r="H22" s="44">
         <v>35912</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>43</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>210</v>
-      </c>
-      <c r="K22" s="25" t="s">
-        <v>211</v>
+        <v>207</v>
+      </c>
+      <c r="K22" s="24" t="s">
+        <v>208</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M22" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N22" s="24" t="s">
+      <c r="N22" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O22" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q22" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="R22" s="2"/>
+      <c r="S22" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="P22" s="2" t="s">
+      <c r="T22" s="27" t="s">
         <v>214</v>
-      </c>
-      <c r="Q22" s="4" t="s">
-        <v>215</v>
-      </c>
-      <c r="R22" s="2"/>
-      <c r="S22" s="25" t="s">
-        <v>216</v>
-      </c>
-      <c r="T22" s="28" t="s">
-        <v>217</v>
       </c>
       <c r="U22" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V22" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="W22" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="X22" s="2">
         <v>2021</v>
       </c>
       <c r="Y22" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="Z22" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
     </row>
     <row r="23" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3563,7 +3560,7 @@
         <v>28</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C23" s="4" t="str">
         <f>D23 &amp; COUNTIF(D$2:D23,D23)</f>
@@ -3574,61 +3571,61 @@
         <v>satrio</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>205</v>
-      </c>
-      <c r="F23" s="45">
+        <v>202</v>
+      </c>
+      <c r="F23" s="44">
         <v>45306</v>
       </c>
       <c r="G23" s="17"/>
-      <c r="H23" s="45">
+      <c r="H23" s="44">
         <v>34574</v>
       </c>
       <c r="I23" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="J23" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="K23" s="24" t="s">
+        <v>220</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>221</v>
-      </c>
-      <c r="J23" s="25" t="s">
-        <v>222</v>
-      </c>
-      <c r="K23" s="25" t="s">
-        <v>223</v>
-      </c>
-      <c r="L23" s="4" t="s">
-        <v>224</v>
       </c>
       <c r="M23" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N23" s="24" t="s">
+      <c r="N23" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
-      <c r="S23" s="25" t="s">
+      <c r="S23" s="24" t="s">
+        <v>222</v>
+      </c>
+      <c r="T23" s="27" t="s">
+        <v>223</v>
+      </c>
+      <c r="U23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V23" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="W23" s="3" t="s">
         <v>225</v>
-      </c>
-      <c r="T23" s="28" t="s">
-        <v>226</v>
-      </c>
-      <c r="U23" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="V23" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="W23" s="3" t="s">
-        <v>228</v>
       </c>
       <c r="X23" s="2">
         <v>2012</v>
       </c>
       <c r="Y23" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="Z23" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
     </row>
     <row r="24" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3636,7 +3633,7 @@
         <v>29</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C24" s="4" t="str">
         <f>D24 &amp; COUNTIF(D$2:D24,D24)</f>
@@ -3647,57 +3644,57 @@
         <v>vebi</v>
       </c>
       <c r="E24" s="16" t="s">
-        <v>207</v>
-      </c>
-      <c r="F24" s="45">
+        <v>204</v>
+      </c>
+      <c r="F24" s="44">
         <v>45323</v>
       </c>
       <c r="G24" s="17"/>
-      <c r="H24" s="45">
+      <c r="H24" s="44">
         <v>35110</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="J24" s="25" t="s">
-        <v>230</v>
-      </c>
-      <c r="K24" s="25" t="s">
-        <v>231</v>
+        <v>58</v>
+      </c>
+      <c r="J24" s="24" t="s">
+        <v>227</v>
+      </c>
+      <c r="K24" s="24" t="s">
+        <v>228</v>
       </c>
       <c r="L24" s="4"/>
       <c r="M24" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N24" s="24" t="s">
+      <c r="N24" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-      <c r="S24" s="25" t="s">
-        <v>232</v>
-      </c>
-      <c r="T24" s="28"/>
+      <c r="S24" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="T24" s="27"/>
       <c r="U24" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V24" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="W24" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="X24" s="2">
         <v>2013</v>
       </c>
       <c r="Y24" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="Z24" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="25" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3705,7 +3702,7 @@
         <v>30</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C25" s="4" t="str">
         <f>D25 &amp; COUNTIF(D$2:D25,D25)</f>
@@ -3716,65 +3713,65 @@
         <v>muhammad</v>
       </c>
       <c r="E25" s="16" t="s">
-        <v>209</v>
-      </c>
-      <c r="F25" s="45">
+        <v>206</v>
+      </c>
+      <c r="F25" s="44">
         <v>45362</v>
       </c>
       <c r="G25" s="17"/>
-      <c r="H25" s="45">
+      <c r="H25" s="44">
         <v>34988</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J25" s="25" t="s">
-        <v>235</v>
-      </c>
-      <c r="K25" s="25" t="s">
-        <v>236</v>
+      <c r="J25" s="24" t="s">
+        <v>232</v>
+      </c>
+      <c r="K25" s="24" t="s">
+        <v>233</v>
       </c>
       <c r="L25" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="M25" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N25" s="24" t="s">
+      <c r="N25" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O25" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
-      <c r="S25" s="25" t="s">
+      <c r="S25" s="24" t="s">
+        <v>237</v>
+      </c>
+      <c r="T25" s="27" t="s">
+        <v>238</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="V25" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="T25" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="U25" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="V25" s="3" t="s">
-        <v>243</v>
-      </c>
       <c r="W25" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="X25" s="2">
         <v>2013</v>
       </c>
       <c r="Y25" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="Z25" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="26" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3782,7 +3779,7 @@
         <v>32</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C26" s="4" t="str">
         <f>D26 &amp; COUNTIF(D$2:D26,D26)</f>
@@ -3793,42 +3790,42 @@
         <v>hendy</v>
       </c>
       <c r="E26" s="16" t="s">
-        <v>246</v>
-      </c>
-      <c r="F26" s="45">
+        <v>243</v>
+      </c>
+      <c r="F26" s="44">
         <v>45404</v>
       </c>
       <c r="G26" s="17"/>
-      <c r="H26" s="45">
+      <c r="H26" s="44">
         <v>31316</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J26" s="25" t="s">
-        <v>257</v>
-      </c>
-      <c r="K26" s="25" t="s">
-        <v>258</v>
+      <c r="J26" s="24" t="s">
+        <v>254</v>
+      </c>
+      <c r="K26" s="24" t="s">
+        <v>255</v>
       </c>
       <c r="L26" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="M26" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N26" s="24" t="s">
+      <c r="N26" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
-      <c r="S26" s="25" t="s">
-        <v>260</v>
-      </c>
-      <c r="T26" s="28"/>
+      <c r="S26" s="24" t="s">
+        <v>257</v>
+      </c>
+      <c r="T26" s="27"/>
       <c r="U26" s="2" t="s">
         <v>24</v>
       </c>
@@ -3836,10 +3833,10 @@
       <c r="W26" s="3"/>
       <c r="X26" s="2"/>
       <c r="Y26" s="3" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="Z26" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
     </row>
     <row r="27" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3847,7 +3844,7 @@
         <v>33</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C27" s="4" t="str">
         <f>D27 &amp; COUNTIF(D$2:D27,D27)</f>
@@ -3858,61 +3855,61 @@
         <v>wahyu</v>
       </c>
       <c r="E27" s="16" t="s">
-        <v>248</v>
-      </c>
-      <c r="F27" s="45">
+        <v>245</v>
+      </c>
+      <c r="F27" s="44">
         <v>45444</v>
       </c>
       <c r="G27" s="17"/>
-      <c r="H27" s="45">
+      <c r="H27" s="44">
         <v>35686</v>
       </c>
       <c r="I27" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="J27" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="K27" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="L27" s="4" t="s">
         <v>262</v>
-      </c>
-      <c r="J27" s="25" t="s">
-        <v>263</v>
-      </c>
-      <c r="K27" s="25" t="s">
-        <v>264</v>
-      </c>
-      <c r="L27" s="4" t="s">
-        <v>265</v>
       </c>
       <c r="M27" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N27" s="24" t="s">
+      <c r="N27" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
-      <c r="S27" s="25" t="s">
-        <v>266</v>
-      </c>
-      <c r="T27" s="28" t="s">
-        <v>267</v>
+      <c r="S27" s="24" t="s">
+        <v>263</v>
+      </c>
+      <c r="T27" s="27" t="s">
+        <v>264</v>
       </c>
       <c r="U27" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V27" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="W27" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="X27" s="2">
         <v>2015</v>
       </c>
       <c r="Y27" s="3" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="Z27" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="28" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -3920,7 +3917,7 @@
         <v>34</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="C28" s="4" t="str">
         <f>D28 &amp; COUNTIF(D$2:D28,D28)</f>
@@ -3931,69 +3928,69 @@
         <v>reyhan</v>
       </c>
       <c r="E28" s="16" t="s">
-        <v>250</v>
-      </c>
-      <c r="F28" s="45">
+        <v>247</v>
+      </c>
+      <c r="F28" s="44">
         <v>45433</v>
       </c>
       <c r="G28" s="17"/>
-      <c r="H28" s="45">
+      <c r="H28" s="44">
         <v>35105</v>
       </c>
       <c r="I28" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J28" s="25" t="s">
-        <v>270</v>
-      </c>
-      <c r="K28" s="25" t="s">
-        <v>271</v>
+      <c r="J28" s="24" t="s">
+        <v>267</v>
+      </c>
+      <c r="K28" s="24" t="s">
+        <v>268</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="M28" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N28" s="24" t="s">
+      <c r="N28" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
-      <c r="S28" s="25" t="s">
-        <v>273</v>
-      </c>
-      <c r="T28" s="28" t="s">
-        <v>274</v>
+      <c r="S28" s="24" t="s">
+        <v>270</v>
+      </c>
+      <c r="T28" s="27" t="s">
+        <v>271</v>
       </c>
       <c r="U28" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V28" s="3" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="W28" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="X28" s="2">
         <v>2015</v>
       </c>
       <c r="Y28" s="3" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="Z28" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
     </row>
     <row r="29" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="29">
+      <c r="A29" s="28">
         <v>35</v>
       </c>
-      <c r="B29" s="30" t="s">
-        <v>251</v>
+      <c r="B29" s="29" t="s">
+        <v>248</v>
       </c>
       <c r="C29" s="4" t="str">
         <f>D29 &amp; COUNTIF(D$2:D29,D29)</f>
@@ -4003,60 +4000,60 @@
         <f t="shared" si="0"/>
         <v>anindia</v>
       </c>
-      <c r="E29" s="31" t="s">
-        <v>252</v>
-      </c>
-      <c r="F29" s="46">
+      <c r="E29" s="30" t="s">
+        <v>249</v>
+      </c>
+      <c r="F29" s="45">
         <v>45494</v>
       </c>
-      <c r="G29" s="32"/>
-      <c r="H29" s="46">
+      <c r="G29" s="31"/>
+      <c r="H29" s="45">
         <v>38769</v>
       </c>
-      <c r="I29" s="29" t="s">
+      <c r="I29" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="J29" s="33" t="s">
-        <v>277</v>
-      </c>
-      <c r="K29" s="33" t="s">
-        <v>278</v>
-      </c>
-      <c r="L29" s="29"/>
+      <c r="J29" s="32" t="s">
+        <v>274</v>
+      </c>
+      <c r="K29" s="32" t="s">
+        <v>275</v>
+      </c>
+      <c r="L29" s="28"/>
       <c r="M29" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N29" s="34" t="s">
+      <c r="N29" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="O29" s="29"/>
-      <c r="P29" s="29"/>
-      <c r="Q29" s="29"/>
-      <c r="R29" s="29"/>
-      <c r="S29" s="33" t="s">
-        <v>279</v>
-      </c>
-      <c r="T29" s="35" t="s">
-        <v>280</v>
-      </c>
-      <c r="U29" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="V29" s="36" t="s">
-        <v>191</v>
-      </c>
-      <c r="W29" s="36" t="s">
-        <v>75</v>
-      </c>
-      <c r="X29" s="29">
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
+      <c r="Q29" s="28"/>
+      <c r="R29" s="28"/>
+      <c r="S29" s="32" t="s">
+        <v>276</v>
+      </c>
+      <c r="T29" s="34" t="s">
+        <v>277</v>
+      </c>
+      <c r="U29" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="V29" s="35" t="s">
+        <v>188</v>
+      </c>
+      <c r="W29" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="X29" s="28">
         <v>2023</v>
       </c>
-      <c r="Y29" s="36" t="s">
-        <v>281</v>
+      <c r="Y29" s="35" t="s">
+        <v>278</v>
       </c>
       <c r="Z29" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
     </row>
     <row r="30" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -4064,7 +4061,7 @@
         <v>36</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C30" s="4" t="str">
         <f>D30 &amp; COUNTIF(D$2:D30,D30)</f>
@@ -4075,59 +4072,59 @@
         <v>rachelia</v>
       </c>
       <c r="E30" s="16" t="s">
-        <v>254</v>
-      </c>
-      <c r="F30" s="45">
+        <v>251</v>
+      </c>
+      <c r="F30" s="44">
         <v>45494</v>
       </c>
       <c r="G30" s="17"/>
-      <c r="H30" s="45">
+      <c r="H30" s="44">
         <v>38906</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J30" s="25" t="s">
-        <v>282</v>
-      </c>
-      <c r="K30" s="25" t="s">
-        <v>283</v>
+      <c r="J30" s="24" t="s">
+        <v>279</v>
+      </c>
+      <c r="K30" s="24" t="s">
+        <v>280</v>
       </c>
       <c r="L30" s="2"/>
       <c r="M30" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N30" s="24" t="s">
+      <c r="N30" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
-      <c r="S30" s="25" t="s">
-        <v>284</v>
-      </c>
-      <c r="T30" s="28" t="s">
-        <v>285</v>
+      <c r="S30" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="T30" s="27" t="s">
+        <v>282</v>
       </c>
       <c r="U30" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V30" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="W30" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="X30" s="2">
         <v>2024</v>
       </c>
       <c r="Y30" s="3" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="Z30" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="31" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -4135,7 +4132,7 @@
         <v>37</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C31" s="4" t="str">
         <f>D31 &amp; COUNTIF(D$2:D31,D31)</f>
@@ -4146,65 +4143,65 @@
         <v>atiqah</v>
       </c>
       <c r="E31" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="F31" s="45">
+        <v>253</v>
+      </c>
+      <c r="F31" s="44">
         <v>45494</v>
       </c>
       <c r="G31" s="17"/>
-      <c r="H31" s="45">
+      <c r="H31" s="44">
         <v>38818</v>
       </c>
       <c r="I31" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J31" s="25" t="s">
-        <v>287</v>
-      </c>
-      <c r="K31" s="23"/>
+      <c r="J31" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="K31" s="22"/>
       <c r="L31" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="M31" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N31" s="24" t="s">
+      <c r="N31" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O31" s="2"/>
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
-      <c r="S31" s="25" t="s">
-        <v>289</v>
-      </c>
-      <c r="T31" s="28" t="s">
-        <v>290</v>
+      <c r="S31" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="T31" s="27" t="s">
+        <v>287</v>
       </c>
       <c r="U31" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V31" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="W31" s="3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="X31" s="2">
         <v>2024</v>
       </c>
       <c r="Y31" s="3" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="Z31" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
     </row>
     <row r="32" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="2"/>
       <c r="B32" s="4" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C32" s="4" t="str">
         <f>D32 &amp; COUNTIF(D$2:D32,D32)</f>
@@ -4215,67 +4212,67 @@
         <v>fajar</v>
       </c>
       <c r="E32" s="16" t="s">
+        <v>290</v>
+      </c>
+      <c r="F32" s="44">
+        <v>45459</v>
+      </c>
+      <c r="G32" s="17"/>
+      <c r="H32" s="44">
+        <v>36302</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="K32" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="L32" s="4" t="s">
         <v>293</v>
-      </c>
-      <c r="F32" s="45">
-        <v>45459</v>
-      </c>
-      <c r="G32" s="17"/>
-      <c r="H32" s="45">
-        <v>36302</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>294</v>
-      </c>
-      <c r="K32" s="25" t="s">
-        <v>295</v>
-      </c>
-      <c r="L32" s="4" t="s">
-        <v>296</v>
       </c>
       <c r="M32" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N32" s="24" t="s">
+      <c r="N32" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-      <c r="S32" s="25" t="s">
-        <v>297</v>
-      </c>
-      <c r="T32" s="37" t="s">
-        <v>298</v>
+      <c r="S32" s="24" t="s">
+        <v>294</v>
+      </c>
+      <c r="T32" s="36" t="s">
+        <v>295</v>
       </c>
       <c r="U32" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V32" s="3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="W32" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="X32" s="2">
         <v>2017</v>
       </c>
       <c r="Y32" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="Z32" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
     </row>
     <row r="33" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2"/>
       <c r="B33" s="4" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C33" s="4" t="str">
         <f>D33 &amp; COUNTIF(D$2:D33,D33)</f>
@@ -4286,71 +4283,71 @@
         <v>muhamad</v>
       </c>
       <c r="E33" s="16" t="s">
-        <v>301</v>
-      </c>
-      <c r="F33" s="45">
+        <v>298</v>
+      </c>
+      <c r="F33" s="44">
         <v>45538</v>
       </c>
       <c r="G33" s="17"/>
-      <c r="H33" s="45">
+      <c r="H33" s="44">
         <v>36944</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>43</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="K33" s="25" t="s">
-        <v>303</v>
+        <v>299</v>
+      </c>
+      <c r="K33" s="24" t="s">
+        <v>300</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="M33" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N33" s="24" t="s">
+      <c r="N33" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O33" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
-      <c r="S33" s="25" t="s">
+      <c r="S33" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="T33" s="36" t="s">
+        <v>305</v>
+      </c>
+      <c r="U33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V33" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="W33" s="3" t="s">
         <v>307</v>
-      </c>
-      <c r="T33" s="37" t="s">
-        <v>308</v>
-      </c>
-      <c r="U33" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="V33" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="W33" s="3" t="s">
-        <v>310</v>
       </c>
       <c r="X33" s="2">
         <v>2019</v>
       </c>
       <c r="Y33" s="3" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="Z33" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2"/>
       <c r="B34" s="4" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C34" s="4" t="str">
         <f>D34 &amp; COUNTIF(D$2:D34,D34)</f>
@@ -4361,61 +4358,61 @@
         <v>muhammad</v>
       </c>
       <c r="E34" s="16" t="s">
-        <v>313</v>
-      </c>
-      <c r="F34" s="45">
+        <v>310</v>
+      </c>
+      <c r="F34" s="44">
         <v>45556</v>
       </c>
       <c r="G34" s="17"/>
-      <c r="H34" s="45">
+      <c r="H34" s="44">
         <v>35745</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>315</v>
-      </c>
-      <c r="K34" s="25"/>
+        <v>312</v>
+      </c>
+      <c r="K34" s="24"/>
       <c r="L34" s="4"/>
       <c r="M34" s="19" t="str">
         <f t="shared" si="1"/>
         <v>male</v>
       </c>
-      <c r="N34" s="24" t="s">
+      <c r="N34" s="23" t="s">
         <v>46</v>
       </c>
       <c r="O34" s="4"/>
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
-      <c r="S34" s="25" t="s">
-        <v>316</v>
-      </c>
-      <c r="T34" s="37"/>
+      <c r="S34" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="T34" s="36"/>
       <c r="U34" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V34" s="3" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="W34" s="3" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="X34" s="2">
         <v>2015</v>
       </c>
       <c r="Y34" s="3" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="Z34" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
     </row>
     <row r="35" spans="1:26" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
-      <c r="B35" s="38" t="s">
-        <v>320</v>
+      <c r="B35" s="37" t="s">
+        <v>317</v>
       </c>
       <c r="C35" s="4" t="str">
         <f>D35 &amp; COUNTIF(D$2:D35,D35)</f>
@@ -4426,20 +4423,20 @@
         <v>rino</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F35" s="47">
+        <v>318</v>
+      </c>
+      <c r="F35" s="46">
         <v>45559</v>
       </c>
       <c r="G35" s="6"/>
-      <c r="H35" s="47">
+      <c r="H35" s="46">
         <v>34737</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J35" s="39" t="s">
-        <v>328</v>
+      <c r="J35" s="38" t="s">
+        <v>325</v>
       </c>
       <c r="K35" s="8"/>
       <c r="L35" s="9"/>
@@ -4460,13 +4457,13 @@
       <c r="X35" s="1"/>
       <c r="Y35" s="11"/>
       <c r="Z35" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="36" spans="1:26" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
-      <c r="B36" s="38" t="s">
-        <v>322</v>
+      <c r="B36" s="37" t="s">
+        <v>319</v>
       </c>
       <c r="C36" s="4" t="str">
         <f>D36 &amp; COUNTIF(D$2:D36,D36)</f>
@@ -4477,26 +4474,26 @@
         <v>panca</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="F36" s="47">
+        <v>320</v>
+      </c>
+      <c r="F36" s="46">
         <v>45659</v>
       </c>
       <c r="G36" s="6"/>
-      <c r="H36" s="47">
+      <c r="H36" s="46">
         <v>37124</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J36" s="39" t="s">
-        <v>329</v>
+        <v>93</v>
+      </c>
+      <c r="J36" s="38" t="s">
+        <v>326</v>
       </c>
       <c r="K36" s="8">
         <v>3302052709230000</v>
       </c>
-      <c r="L36" s="40" t="s">
-        <v>330</v>
+      <c r="L36" s="39" t="s">
+        <v>327</v>
       </c>
       <c r="M36" s="19" t="str">
         <f t="shared" si="1"/>
@@ -4509,35 +4506,35 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
-      <c r="S36" s="38" t="s">
-        <v>331</v>
-      </c>
-      <c r="T36" s="41" t="s">
-        <v>332</v>
+      <c r="S36" s="37" t="s">
+        <v>328</v>
+      </c>
+      <c r="T36" s="40" t="s">
+        <v>329</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V36" s="11" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="W36" s="11" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="X36" s="1">
         <v>2019</v>
       </c>
       <c r="Y36" s="11" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="Z36" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="37" spans="1:26" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
-      <c r="B37" s="38" t="s">
-        <v>324</v>
+      <c r="B37" s="37" t="s">
+        <v>321</v>
       </c>
       <c r="C37" s="4" t="str">
         <f>D37 &amp; COUNTIF(D$2:D37,D37)</f>
@@ -4548,26 +4545,26 @@
         <v>muhammad</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="F37" s="47">
+        <v>322</v>
+      </c>
+      <c r="F37" s="46">
         <v>45666</v>
       </c>
       <c r="G37" s="6"/>
-      <c r="H37" s="47">
+      <c r="H37" s="46">
         <v>37755</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="J37" s="39" t="s">
-        <v>335</v>
-      </c>
-      <c r="K37" s="42" t="s">
-        <v>336</v>
-      </c>
-      <c r="L37" s="40" t="s">
-        <v>337</v>
+        <v>175</v>
+      </c>
+      <c r="J37" s="38" t="s">
+        <v>332</v>
+      </c>
+      <c r="K37" s="41" t="s">
+        <v>333</v>
+      </c>
+      <c r="L37" s="39" t="s">
+        <v>334</v>
       </c>
       <c r="M37" s="19" t="str">
         <f t="shared" si="1"/>
@@ -4580,33 +4577,33 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
-      <c r="S37" s="38" t="s">
-        <v>338</v>
+      <c r="S37" s="37" t="s">
+        <v>335</v>
       </c>
       <c r="T37" s="10"/>
       <c r="U37" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V37" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="W37" s="11" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="X37" s="1">
         <v>2021</v>
       </c>
       <c r="Y37" s="11" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="Z37" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="38" spans="1:26" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
-      <c r="B38" s="38" t="s">
-        <v>326</v>
+      <c r="B38" s="37" t="s">
+        <v>323</v>
       </c>
       <c r="C38" s="4" t="str">
         <f>D38 &amp; COUNTIF(D$2:D38,D38)</f>
@@ -4617,26 +4614,26 @@
         <v>aditya</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F38" s="47">
+        <v>324</v>
+      </c>
+      <c r="F38" s="46">
         <v>45680</v>
       </c>
       <c r="G38" s="6"/>
-      <c r="H38" s="47">
+      <c r="H38" s="46">
         <v>38117</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J38" s="39" t="s">
-        <v>342</v>
-      </c>
-      <c r="K38" s="42" t="s">
-        <v>343</v>
-      </c>
-      <c r="L38" s="40" t="s">
-        <v>344</v>
+      <c r="J38" s="38" t="s">
+        <v>339</v>
+      </c>
+      <c r="K38" s="41" t="s">
+        <v>340</v>
+      </c>
+      <c r="L38" s="39" t="s">
+        <v>341</v>
       </c>
       <c r="M38" s="19" t="str">
         <f t="shared" si="1"/>
@@ -4649,68 +4646,68 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" s="38" t="s">
-        <v>345</v>
-      </c>
-      <c r="T38" s="41" t="s">
-        <v>346</v>
+      <c r="S38" s="37" t="s">
+        <v>342</v>
+      </c>
+      <c r="T38" s="40" t="s">
+        <v>343</v>
       </c>
       <c r="U38" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V38" s="11" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="W38" s="11" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="X38" s="1">
         <v>2022</v>
       </c>
       <c r="Y38" s="11" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="Z38" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="39" spans="1:26" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2"/>
       <c r="B39" s="4" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C39" s="4" t="str">
         <f>D39 &amp; COUNTIF(D$2:D39,D39)</f>
         <v>wita1</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>349</v>
-      </c>
-      <c r="F39" s="45">
+        <v>346</v>
+      </c>
+      <c r="F39" s="44">
         <v>45680</v>
       </c>
       <c r="G39" s="17"/>
-      <c r="H39" s="45">
+      <c r="H39" s="44">
         <v>39311</v>
       </c>
       <c r="I39" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J39" s="43" t="s">
-        <v>354</v>
-      </c>
-      <c r="K39" s="25" t="s">
-        <v>355</v>
-      </c>
-      <c r="L39" s="24"/>
+      <c r="J39" s="42" t="s">
+        <v>351</v>
+      </c>
+      <c r="K39" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="L39" s="23"/>
       <c r="M39" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N39" s="24" t="s">
+      <c r="N39" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O39" s="4"/>
@@ -4718,30 +4715,30 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
       <c r="S39" s="4" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="T39" s="16"/>
       <c r="U39" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="V39" s="3" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="W39" s="3"/>
       <c r="X39" s="2">
         <v>2024</v>
       </c>
       <c r="Y39" s="3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="Z39" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="40" spans="1:26" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2"/>
       <c r="B40" s="4" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C40" s="4" t="str">
         <f>D40 &amp; COUNTIF(D$2:D40,D40)</f>
@@ -4752,32 +4749,32 @@
         <v>cameliana</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="F40" s="45">
+        <v>348</v>
+      </c>
+      <c r="F40" s="44">
         <v>45680</v>
       </c>
       <c r="G40" s="17"/>
-      <c r="H40" s="45">
+      <c r="H40" s="44">
         <v>38045</v>
       </c>
       <c r="I40" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J40" s="43" t="s">
-        <v>359</v>
-      </c>
-      <c r="K40" s="25" t="s">
-        <v>360</v>
+      <c r="J40" s="42" t="s">
+        <v>356</v>
+      </c>
+      <c r="K40" s="24" t="s">
+        <v>357</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="M40" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N40" s="24" t="s">
+      <c r="N40" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O40" s="2"/>
@@ -4785,34 +4782,34 @@
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
       <c r="S40" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="T40" s="36" t="s">
+        <v>360</v>
+      </c>
+      <c r="U40" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="V40" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="W40" s="3" t="s">
         <v>362</v>
-      </c>
-      <c r="T40" s="37" t="s">
-        <v>363</v>
-      </c>
-      <c r="U40" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="V40" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="W40" s="3" t="s">
-        <v>365</v>
       </c>
       <c r="X40" s="2">
         <v>2024</v>
       </c>
       <c r="Y40" s="3" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="Z40" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="41" spans="1:26" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
-      <c r="B41" s="38" t="s">
-        <v>352</v>
+      <c r="B41" s="37" t="s">
+        <v>349</v>
       </c>
       <c r="C41" s="4" t="str">
         <f>D41 &amp; COUNTIF(D$2:D41,D41)</f>
@@ -4823,24 +4820,24 @@
         <v>muhamad</v>
       </c>
       <c r="E41" s="11" t="s">
-        <v>353</v>
-      </c>
-      <c r="F41" s="47">
+        <v>350</v>
+      </c>
+      <c r="F41" s="46">
         <v>45699</v>
       </c>
       <c r="G41" s="6"/>
-      <c r="H41" s="47">
+      <c r="H41" s="46">
         <v>38455</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J41" s="39" t="s">
-        <v>367</v>
-      </c>
-      <c r="K41" s="42"/>
-      <c r="L41" s="38" t="s">
-        <v>368</v>
+      <c r="J41" s="38" t="s">
+        <v>364</v>
+      </c>
+      <c r="K41" s="41"/>
+      <c r="L41" s="37" t="s">
+        <v>365</v>
       </c>
       <c r="M41" s="19" t="str">
         <f t="shared" si="1"/>
@@ -4853,35 +4850,35 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
-      <c r="S41" s="38" t="s">
+      <c r="S41" s="37" t="s">
+        <v>366</v>
+      </c>
+      <c r="T41" s="40" t="s">
+        <v>367</v>
+      </c>
+      <c r="U41" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="V41" s="11" t="s">
+        <v>368</v>
+      </c>
+      <c r="W41" s="11" t="s">
         <v>369</v>
-      </c>
-      <c r="T41" s="41" t="s">
-        <v>370</v>
-      </c>
-      <c r="U41" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="V41" s="11" t="s">
-        <v>371</v>
-      </c>
-      <c r="W41" s="11" t="s">
-        <v>372</v>
       </c>
       <c r="X41" s="1">
         <v>2023</v>
       </c>
       <c r="Y41" s="11" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="Z41" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="42" spans="1:26" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2"/>
       <c r="B42" s="4" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="C42" s="4" t="str">
         <f>D42 &amp; COUNTIF(D$2:D42,D42)</f>
@@ -4892,30 +4889,30 @@
         <v>satrio</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="F42" s="45">
+        <v>372</v>
+      </c>
+      <c r="F42" s="44">
         <v>45699</v>
       </c>
       <c r="G42" s="17"/>
-      <c r="H42" s="45">
+      <c r="H42" s="44">
         <v>36578</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="J42" s="43" t="s">
-        <v>376</v>
-      </c>
-      <c r="K42" s="25" t="s">
-        <v>377</v>
-      </c>
-      <c r="L42" s="24"/>
+        <v>259</v>
+      </c>
+      <c r="J42" s="42" t="s">
+        <v>373</v>
+      </c>
+      <c r="K42" s="24" t="s">
+        <v>374</v>
+      </c>
+      <c r="L42" s="23"/>
       <c r="M42" s="19" t="str">
         <f t="shared" si="1"/>
         <v>female</v>
       </c>
-      <c r="N42" s="24" t="s">
+      <c r="N42" s="23" t="s">
         <v>23</v>
       </c>
       <c r="O42" s="2"/>
@@ -4923,28 +4920,28 @@
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
       <c r="S42" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="T42" s="37" t="s">
-        <v>379</v>
+        <v>375</v>
+      </c>
+      <c r="T42" s="36" t="s">
+        <v>376</v>
       </c>
       <c r="U42" s="2" t="s">
         <v>24</v>
       </c>
       <c r="V42" s="3" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="W42" s="3" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="X42" s="2">
         <v>2023</v>
       </c>
       <c r="Y42" s="3" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="Z42" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>